<commit_message>
Feito 1 e 2
</commit_message>
<xml_diff>
--- a/Exercicios_Dart.xlsx
+++ b/Exercicios_Dart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programação\DART\Exercicios Eric\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programação\DART\Exercicios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9058A75-3EFB-41B6-988F-803513AF7A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429B1BAB-E73C-4545-A0BB-EFCE0810A765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -539,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,6 +564,9 @@
       <c r="B2" t="s">
         <v>22</v>
       </c>
+      <c r="C2" s="2" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -571,6 +574,9 @@
       </c>
       <c r="B3" t="s">
         <v>23</v>
+      </c>
+      <c r="C3" s="2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>